<commit_message>
added user magement section
</commit_message>
<xml_diff>
--- a/uploads/Test.xlsx
+++ b/uploads/Test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BBBBC5-D7EE-43D5-A22E-F148C096F314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03389C5-3C61-460C-A0FA-4954F3F2F2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Id</t>
   </si>
@@ -52,19 +52,28 @@
   </si>
   <si>
     <t>Kac</t>
+  </si>
+  <si>
+    <t>good</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,8 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,30 +381,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="2.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -403,7 +415,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -414,7 +426,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -425,24 +437,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added search and fix ather updates
</commit_message>
<xml_diff>
--- a/uploads/Test.xlsx
+++ b/uploads/Test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03389C5-3C61-460C-A0FA-4954F3F2F2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F5AD53-CD60-4522-AB8F-5781CDC55561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Id</t>
   </si>
@@ -55,6 +56,24 @@
   </si>
   <si>
     <t>good</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>khalif</t>
+  </si>
+  <si>
+    <t>KHALIF</t>
+  </si>
+  <si>
+    <t>HaYe</t>
+  </si>
+  <si>
+    <t>yaah</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -381,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -462,7 +481,51 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7811ACBD-C97A-4687-B4DE-A28ECAC7815F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>